<commit_message>
Adding Assertion Request Json
</commit_message>
<xml_diff>
--- a/src/test/java/tests/requestResponseValidation/model/TestcaseSNAPBI.xlsx
+++ b/src/test/java/tests/requestResponseValidation/model/TestcaseSNAPBI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSP\Automation-Testing\Disbursement-Testing\api-client-testing\src\test\java\tests\requestResponseValidation\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91EEFE1-2500-4A0A-BF6F-45ABBB8A52EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ED1ED7-52B9-4A9D-BB3B-E7AAF6335EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="122">
   <si>
     <t>No</t>
   </si>
@@ -289,36 +289,6 @@
     <t xml:space="preserve">Tanggal Pengujian: </t>
   </si>
   <si>
-    <t>Request 3</t>
-  </si>
-  <si>
-    <t>Response 3</t>
-  </si>
-  <si>
-    <t>Request 4</t>
-  </si>
-  <si>
-    <t>Response 4</t>
-  </si>
-  <si>
-    <t>Request 5</t>
-  </si>
-  <si>
-    <t>Response 5</t>
-  </si>
-  <si>
-    <t>Request 6</t>
-  </si>
-  <si>
-    <t>Response 6</t>
-  </si>
-  <si>
-    <t>Request 7</t>
-  </si>
-  <si>
-    <t>Response 7</t>
-  </si>
-  <si>
     <t>Request 8</t>
   </si>
   <si>
@@ -373,18 +343,6 @@
     <t>Response 16</t>
   </si>
   <si>
-    <t>Request 17</t>
-  </si>
-  <si>
-    <t>Response 17</t>
-  </si>
-  <si>
-    <t>Request 18</t>
-  </si>
-  <si>
-    <t>Response 18</t>
-  </si>
-  <si>
     <t>Request 19</t>
   </si>
   <si>
@@ -395,24 +353,6 @@
   </si>
   <si>
     <t>Response 20</t>
-  </si>
-  <si>
-    <t>Request 21</t>
-  </si>
-  <si>
-    <t>Response 21</t>
-  </si>
-  <si>
-    <t>Request 22</t>
-  </si>
-  <si>
-    <t>Response 22</t>
-  </si>
-  <si>
-    <t>Request 23</t>
-  </si>
-  <si>
-    <t>Response 23</t>
   </si>
   <si>
     <t>{
@@ -474,6 +414,155 @@
   </si>
   <si>
     <t>{"responseMessage":"Conflict","responseCode":"4094700"}</t>
+  </si>
+  <si>
+    <t>{
+	"X-TIMESTAMP": "2024-06-20T11:25:49+07:00",
+	"X-SIGNATURE": "uwmeyLSYrBYSIDj7p3uugvVmJd8+j4B+33Pa2vimEEGhr/dPZBEXgTGyn/eH3+2g3mkwKcjweB5jQJxKV602ZQ==",
+	"X-EXTERNAL-ID": "4062011259742597360",
+	"X-PARTNER-ID": "0636ea90-829e-11ee-aca0-e3c0230e65f9",
+	"CHANNEL-ID": "INDIVARA",
+	"X-DEVICE-ID": "Mozilla"
+}
+{
+	"merchantId": "998023046964160",
+	"terminalId": "DSP00001",
+	"amount": {
+		"value": "15001.00",
+		"currency": "IDR"
+	},
+	"additionalInfo": {
+		"productType": "Purchase",
+		"isWebview": false,
+		"billingId": ""
+	},
+	"validityPeriod": "2024-06-21T11:25:17+07:00",
+	"callbackUrl": ""
+}</t>
+  </si>
+  <si>
+    <t>{"responseMessage":"Invalid Mandatory Field  [Missing partnerReferenceNo]","responseCode":"4004702"}</t>
+  </si>
+  <si>
+    <t>{"X-TIMESTAMP":"2024-06-26T16:52:58+07:00","X-SIGNATURE":"rdKPTioqBk2h5Iww/lpOCsDP7BtrtmEOIRukhZ9c065yiQpMuICKOP9yKX7nQD2P5votSPRKzNfJzEe7H8mKjQ==","X-EXTERNAL-ID":"4062616536089790864","X-PARTNER-ID":"0636ea90-829e-11ee-aca0-e3c0230e65f9","CHANNEL-ID":"INDIVARA","X-DEVICE-ID":"Mozilla"}
+{"partnerReferenceNo":"24062616526905706716","merchantId":"998023046964160","terminalId":"DSPPPPPPPPPPPPPPPPPPPPPPPPPPPPP00001","amount":{"currency":"IDR","value":"15001.00"},"additionalInfo":{"productType":"Purchase","isWebview":false,"billingId":""},"validityPeriod":"2024-06-26T23:34:00+07:00","callbackUrl":""}</t>
+  </si>
+  <si>
+    <t>{"responseMessage":"Invalid Field Format  [Max terminalId length is 8]","responseCode":"4004701"}</t>
+  </si>
+  <si>
+    <t>{
+	"X-TIMESTAMP": "2024-07-09T09:32:21+07:00",
+	"X-SIGNATURE": "yxzflDsGPKMh4AlCLdsXH5cOvylO9y981hpZ7IT0O7VIyXtkusGNzmqWwInaGXoGlsXToVRXPWGPkWi+gfq6vg==",
+	"X-EXTERNAL-ID": "4070909326588547036",
+	"X-PARTNER-ID": "0636ea90-829e-11ee-aca0-e3c0230e65f9",
+	"CHANNEL-ID": "INDIVARA",
+	"X-DEVICE-ID": "Mozilla"
+}
+{
+	"partnerReferenceNo": "24070909321934786676",
+	"merchantId": "998023046964160",
+	"terminalId": "DSP00001",
+	"amount": {
+		"value": "10002.00",
+		"currency": "IDR"
+	},
+	"additionalInfo": {
+		"productType": "remoteQR",
+		"isWebview": false,
+		"billingId": ""
+	},
+	"validityPeriod": "2024-07-09T17:51:00+07:00",
+	"callbackUrl": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+	"qrContent": "00020101021226710019ID.CO.DSPRATAMA.WWW011893600998000000823502159980230469641600303UBE51440014ID.CO.QRIS.WWW0215ID12345678912340303UBE5204829953033605405100025802ID5908INDIVARA6007Jakarta61051424062780708DSP0000150620002000102100204000803040386041639C7E4539366CFC8051007090932476304C1E1",
+	"additionalInfo": {
+		"transactionHash": "CFDDBCD258101F394D0EA52A889C463AC6EEC6B97398743CCEB754D916FB4B93"
+	},
+	"partnerReferenceNo": "24070909321934786676",
+	"responseMessage": "Successful",
+	"responseCode": "2004700"
+}</t>
+  </si>
+  <si>
+    <t>{
+	"X-TIMESTAMP": "2024-06-20T11:42:08+07:00",
+	"X-SIGNATURE": "mQqQbXxIr+7A7EIG4lr/Q2QvMqcV6qqC4dxfpr6XM/beuFiEZcLdgokE7GhTID5F2pD3ZWdRI3ABBYSpkcWgJQ==",
+	"X-EXTERNAL-ID": "4062011429215169645",
+	"X-PARTNER-ID": "0636ea90-829e-11ee-aca0-e3c0230e65f9",
+	"CHANNEL-ID": "INDIVARA",
+	"X-DEVICE-ID": "Mozilla"
+}
+{
+	"partnerReferenceNo": "24062011414045706183",
+	"merchantId": "998023046964161",
+	"terminalId": "DSP00001",
+	"amount": {
+		"value": "15001.00",
+		"currency": "IDR"
+	},
+	"additionalInfo": {
+		"productType": "Purchase",
+		"isWebview": "false",
+		"billingId": ""
+	},
+	"validityPeriod": "2024-06-21T11:41:05+07:00",
+	"callbackUrl": ""
+}</t>
+  </si>
+  <si>
+    <t>{"responseMessage":"Invalid Merchant","responseCode":"4044708"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {"amount":{"value":"10002.00","currency":"IDR"},"originalReferenceNo":"421912128500","latestTransactionStatus":"00","additionalInfo":{"invoiceNumber":"76025920377602592037","merchantData":{"mpan":"9360099800000082358","merchantId":"998023046964160","terminalId":"DSP00001"},"transactionDate":"2024-08-06T12:12:21+07:00","transactionHash":"56E531C0A80981715A74093DB5D1A656D0D8846653DBFC7E335B145CE9386541","transactionId":"998023046964160.421912128500.0806121221","issuerData":{"cPan":"9360012519770301004","issInsCode":"125","issInsName":"BANK KALTENG"}},"originalPartnerReferenceNo":"24080612094706406722","transactionStatusDesc":"PURCHASE_APPROVED"}</t>
+  </si>
+  <si>
+    <t>{"responseCode":"2005200","responseMessage":"success"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {"amount":{"currency":"IDR","value":"15001.00"},"originalReferenceNo":"417816357219","latestTransactionStatus":"06","additionalInfo":{"invoiceNumber":null,"merchantData":{"mpan":"9360099800000082358","merchantId":"998023046964160","terminalId":"DSP00001"},"transactionDate":"2024-06-26T16:36:07+07:00","transactionHash":"46667F28478F67A61DABB93AB46FEF1CB4DD4B2B5852C40F28AC19628D2CCA77","transactionId":"998023046964160.417816357219.0626163556","issuerData":{"cPan":"9360012519770301004","issInsCode":"125","issInsName":"BANK KALTENG"}},"originalPartnerReferenceNo":"24062616320319215260","transactionStatusDesc":"PURCHASE_DECLINED"}</t>
+  </si>
+  <si>
+    <t>{"partnerRefundNo":"RF240920150634062813","originalPartnerReferenceNo":"24092015044143485815","originalReferenceNo":"426415058948","originalExternalId":"4092015048860996441","merchantId":"998023046964160","refundAmount":{"value":"10004.00","currency":"IDR"},"reason":"Customer request"}</t>
+  </si>
+  <si>
+    <t>{"originalReferenceNo":"426415058948","referenceNo":"756264027557","originalExternalId":"4092015048860996441","refundTime":"2024-09-20T15:06:29+07:00","originalPartnerReferenceNo":"24092015044143485815","responseMessage":"Successful","partnerRefundNo":"RF240920150634062813","refundAmount":{"value":"10004.00","currency":"IDR"},"responseCode":"2007800"}</t>
+  </si>
+  <si>
+    <t>{"partnerRefundNo": "RF240925141106906949",
+	"originalPartnerReferenceNo": "24092514100495848840",
+	"originalReferenceNo": "426914108998",
+	"originalExternalId": "4092514105531900497",
+	"merchantId": "998023046964160",
+	"refundAmount": {
+		"value": "10001.00",
+		"currency": "IDR"
+	},
+	"reason": "Customer request"}</t>
+  </si>
+  <si>
+    <t>{"originalReferenceNo": "426914108998",
+	"referenceNo": "203457319894",
+	"originalExternalId": "4092514105531900497",
+	"refundTime": "2024-09-25T14:12:13+07:00",
+	"originalPartnerReferenceNo": "24092514100495848840",
+	"responseMessage": "Request In Progress",
+	"partnerRefundNo": "RF240925141106906949",
+	"refundAmount": {
+		"value": "10001.00",
+		"currency": "IDR"
+	},
+	"responseCode": "2027800"}</t>
+  </si>
+  <si>
+    <t>{"X-TIMESTAMP":"2024-06-26T16:38:43+07:00","X-SIGNATURE":"Q1LYGDTpxJSe8BfFtyi7nwZmb4wWM6yWqnl6cxNQsTM62wH37o8CzwCAc43ydFnVQtQs8yf01L9KfdG3FyOdow==","X-EXTERNAL-ID":"4062616389916801790","X-PARTNER-ID":"0636ea90-829e-11ee-aca0-e3c0230e65f9","CHANNEL-ID":"INDIVARA","X-DEVICE-ID":"Mozilla"}
+{"originalPartnerReferenceNo":"24062616261149911290","originalExternalId":"4062616261162865911","transactionDate":"2024-06-26T16:26:22+07:00","serviceCode":"47","additionalInfo":{"transactionHash":"0A36BBE355EEBB45C31DBCD6E0D3862A629A6B630E24D9556070AD2CBB951DDF","merchantId":"998023046964160"}}</t>
+  </si>
+  <si>
+    <t>{"amount":{"currency":"IDR","value":"15001.00"},"originalReferenceNo":"","serviceCode":"47","latestTransactionStatus":"01","additionalInfo":{"transactionType":"PURCHASE","invoiceNumber":null,"merchantData":{"mpan":"9360099800000082358","merchantId":"998023046964160","terminalId":"DSP00001"},"issuerData":{"cPan":"","issInsCode":"","issInsName":""},"transactionHash":"0A36BBE355EEBB45C31DBCD6E0D3862A629A6B630E24D9556070AD2CBB951DDF"},"transactionStatusDesc":"PURCHASE_INIT","originalPartnerReferenceNo":"24062616261149911290","transactionDate":"2024-06-26T16:26:23+07:00","responseMessage":"Successful","responseCode":"2005300"}</t>
   </si>
 </sst>
 </file>
@@ -598,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -649,11 +738,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -877,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.75" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -896,12 +988,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="5"/>
@@ -991,11 +1083,11 @@
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>121</v>
+      <c r="E10" s="18" t="s">
+        <v>101</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>122</v>
+      <c r="F10" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1031,11 +1123,11 @@
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>123</v>
+      <c r="E11" s="18" t="s">
+        <v>103</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>124</v>
+      <c r="F11" s="18" t="s">
+        <v>104</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1072,10 +1164,10 @@
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>80</v>
+      <c r="F12" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1112,10 +1204,10 @@
         <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>82</v>
+      <c r="F13" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1152,10 +1244,10 @@
         <v>52</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>84</v>
+      <c r="F14" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1192,10 +1284,10 @@
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>86</v>
+      <c r="F15" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1232,10 +1324,10 @@
         <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>88</v>
+      <c r="F16" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1272,10 +1364,10 @@
         <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1312,10 +1404,10 @@
         <v>29</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1352,10 +1444,10 @@
         <v>32</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1392,10 +1484,10 @@
         <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1432,10 +1524,10 @@
         <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1472,10 +1564,10 @@
         <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1512,10 +1604,10 @@
         <v>39</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1552,10 +1644,10 @@
         <v>41</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1592,10 +1684,10 @@
         <v>44</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1632,10 +1724,10 @@
         <v>46</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1671,11 +1763,11 @@
       <c r="D27" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>109</v>
+      <c r="E27" s="11" t="s">
+        <v>115</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>110</v>
+      <c r="F27" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -1712,10 +1804,10 @@
         <v>66</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1752,10 +1844,10 @@
         <v>68</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1792,10 +1884,10 @@
         <v>71</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1832,10 +1924,10 @@
         <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1871,11 +1963,11 @@
       <c r="D32" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>119</v>
+      <c r="E32" s="12" t="s">
+        <v>120</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>120</v>
+      <c r="F32" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="12"/>

</xml_diff>